<commit_message>
Small statistics xls fixes
</commit_message>
<xml_diff>
--- a/public/xls-template/Statistik.xlsx
+++ b/public/xls-template/Statistik.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evikomp" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -66,8 +66,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,9 +91,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -95,10 +121,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -383,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -397,72 +447,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="6"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="10" t="s">
         <v>6</v>
       </c>
     </row>
@@ -470,6 +520,11 @@
       <c r="A3" s="1">
         <v>44166</v>
       </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3"/>
       <c r="K3">
         <f>I3+J3</f>
         <v>0</v>
@@ -478,7 +533,9 @@
         <f>SUM(K$3:K3)</f>
         <v>0</v>
       </c>
-      <c r="O3">
+      <c r="M3" s="4"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3">
         <f>SUM(N$3:N3)</f>
         <v>0</v>
       </c>
@@ -487,6 +544,11 @@
       <c r="A4" s="1">
         <v>44197</v>
       </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
       <c r="K4">
         <f t="shared" ref="K4:K26" si="0">I4+J4</f>
         <v>0</v>
@@ -495,7 +557,9 @@
         <f>SUM(K$3:K4)</f>
         <v>0</v>
       </c>
-      <c r="O4">
+      <c r="M4" s="4"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3">
         <f>SUM(N$3:N4)</f>
         <v>0</v>
       </c>
@@ -504,6 +568,11 @@
       <c r="A5" s="1">
         <v>44228</v>
       </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
       <c r="K5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -512,7 +581,9 @@
         <f>SUM(K$3:K5)</f>
         <v>0</v>
       </c>
-      <c r="O5">
+      <c r="M5" s="4"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3">
         <f>SUM(N$3:N5)</f>
         <v>0</v>
       </c>
@@ -521,6 +592,11 @@
       <c r="A6" s="1">
         <v>44256</v>
       </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="3"/>
       <c r="K6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -529,7 +605,9 @@
         <f>SUM(K$3:K6)</f>
         <v>0</v>
       </c>
-      <c r="O6">
+      <c r="M6" s="4"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3">
         <f>SUM(N$3:N6)</f>
         <v>0</v>
       </c>
@@ -538,6 +616,11 @@
       <c r="A7" s="1">
         <v>44287</v>
       </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
       <c r="K7">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -546,7 +629,9 @@
         <f>SUM(K$3:K7)</f>
         <v>0</v>
       </c>
-      <c r="O7">
+      <c r="M7" s="4"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="3">
         <f>SUM(N$3:N7)</f>
         <v>0</v>
       </c>
@@ -555,6 +640,11 @@
       <c r="A8" s="1">
         <v>44317</v>
       </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="3"/>
       <c r="K8">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -563,7 +653,9 @@
         <f>SUM(K$3:K8)</f>
         <v>0</v>
       </c>
-      <c r="O8">
+      <c r="M8" s="4"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3">
         <f>SUM(N$3:N8)</f>
         <v>0</v>
       </c>
@@ -572,6 +664,11 @@
       <c r="A9" s="1">
         <v>44348</v>
       </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="3"/>
       <c r="K9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -580,7 +677,9 @@
         <f>SUM(K$3:K9)</f>
         <v>0</v>
       </c>
-      <c r="O9">
+      <c r="M9" s="4"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="3">
         <f>SUM(N$3:N9)</f>
         <v>0</v>
       </c>
@@ -589,6 +688,11 @@
       <c r="A10" s="1">
         <v>44378</v>
       </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="3"/>
       <c r="K10">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -597,7 +701,9 @@
         <f>SUM(K$3:K10)</f>
         <v>0</v>
       </c>
-      <c r="O10">
+      <c r="M10" s="4"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="3">
         <f>SUM(N$3:N10)</f>
         <v>0</v>
       </c>
@@ -606,6 +712,11 @@
       <c r="A11" s="1">
         <v>44409</v>
       </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="3"/>
       <c r="K11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -614,7 +725,9 @@
         <f>SUM(K$3:K11)</f>
         <v>0</v>
       </c>
-      <c r="O11">
+      <c r="M11" s="4"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="3">
         <f>SUM(N$3:N11)</f>
         <v>0</v>
       </c>
@@ -623,6 +736,11 @@
       <c r="A12" s="1">
         <v>44440</v>
       </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="3"/>
       <c r="K12">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -631,7 +749,9 @@
         <f>SUM(K$3:K12)</f>
         <v>0</v>
       </c>
-      <c r="O12">
+      <c r="M12" s="4"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="3">
         <f>SUM(N$3:N12)</f>
         <v>0</v>
       </c>
@@ -640,6 +760,11 @@
       <c r="A13" s="1">
         <v>44470</v>
       </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
       <c r="K13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -648,7 +773,9 @@
         <f>SUM(K$3:K13)</f>
         <v>0</v>
       </c>
-      <c r="O13">
+      <c r="M13" s="4"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="3">
         <f>SUM(N$3:N13)</f>
         <v>0</v>
       </c>
@@ -657,6 +784,11 @@
       <c r="A14" s="1">
         <v>44501</v>
       </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="3"/>
       <c r="K14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -665,7 +797,9 @@
         <f>SUM(K$3:K14)</f>
         <v>0</v>
       </c>
-      <c r="O14">
+      <c r="M14" s="4"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="3">
         <f>SUM(N$3:N14)</f>
         <v>0</v>
       </c>
@@ -674,6 +808,11 @@
       <c r="A15" s="1">
         <v>44531</v>
       </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="3"/>
       <c r="K15">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -682,7 +821,9 @@
         <f>SUM(K$3:K15)</f>
         <v>0</v>
       </c>
-      <c r="O15">
+      <c r="M15" s="4"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="3">
         <f>SUM(N$3:N15)</f>
         <v>0</v>
       </c>
@@ -691,6 +832,11 @@
       <c r="A16" s="1">
         <v>44562</v>
       </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
       <c r="K16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -699,7 +845,9 @@
         <f>SUM(K$3:K16)</f>
         <v>0</v>
       </c>
-      <c r="O16">
+      <c r="M16" s="4"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="3">
         <f>SUM(N$3:N16)</f>
         <v>0</v>
       </c>
@@ -708,6 +856,11 @@
       <c r="A17" s="1">
         <v>44593</v>
       </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
       <c r="K17">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -716,7 +869,9 @@
         <f>SUM(K$3:K17)</f>
         <v>0</v>
       </c>
-      <c r="O17">
+      <c r="M17" s="4"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="3">
         <f>SUM(N$3:N17)</f>
         <v>0</v>
       </c>
@@ -725,6 +880,11 @@
       <c r="A18" s="1">
         <v>44621</v>
       </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
       <c r="K18">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -733,7 +893,9 @@
         <f>SUM(K$3:K18)</f>
         <v>0</v>
       </c>
-      <c r="O18">
+      <c r="M18" s="4"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="3">
         <f>SUM(N$3:N18)</f>
         <v>0</v>
       </c>
@@ -742,6 +904,11 @@
       <c r="A19" s="1">
         <v>44652</v>
       </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="3"/>
       <c r="K19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -750,7 +917,9 @@
         <f>SUM(K$3:K19)</f>
         <v>0</v>
       </c>
-      <c r="O19">
+      <c r="M19" s="4"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="3">
         <f>SUM(N$3:N19)</f>
         <v>0</v>
       </c>
@@ -759,6 +928,11 @@
       <c r="A20" s="1">
         <v>44682</v>
       </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
       <c r="K20">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -767,7 +941,9 @@
         <f>SUM(K$3:K20)</f>
         <v>0</v>
       </c>
-      <c r="O20">
+      <c r="M20" s="4"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="3">
         <f>SUM(N$3:N20)</f>
         <v>0</v>
       </c>
@@ -776,6 +952,11 @@
       <c r="A21" s="1">
         <v>44713</v>
       </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="3"/>
       <c r="K21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -784,7 +965,9 @@
         <f>SUM(K$3:K21)</f>
         <v>0</v>
       </c>
-      <c r="O21">
+      <c r="M21" s="4"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="3">
         <f>SUM(N$3:N21)</f>
         <v>0</v>
       </c>
@@ -793,6 +976,11 @@
       <c r="A22" s="1">
         <v>44743</v>
       </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="3"/>
       <c r="K22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -801,7 +989,9 @@
         <f>SUM(K$3:K22)</f>
         <v>0</v>
       </c>
-      <c r="O22">
+      <c r="M22" s="4"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="3">
         <f>SUM(N$3:N22)</f>
         <v>0</v>
       </c>
@@ -810,6 +1000,11 @@
       <c r="A23" s="1">
         <v>44774</v>
       </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="3"/>
       <c r="K23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -818,7 +1013,9 @@
         <f>SUM(K$3:K23)</f>
         <v>0</v>
       </c>
-      <c r="O23">
+      <c r="M23" s="4"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="3">
         <f>SUM(N$3:N23)</f>
         <v>0</v>
       </c>
@@ -827,6 +1024,11 @@
       <c r="A24" s="1">
         <v>44805</v>
       </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="3"/>
       <c r="K24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -835,7 +1037,9 @@
         <f>SUM(K$3:K24)</f>
         <v>0</v>
       </c>
-      <c r="O24">
+      <c r="M24" s="4"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="3">
         <f>SUM(N$3:N24)</f>
         <v>0</v>
       </c>
@@ -844,6 +1048,11 @@
       <c r="A25" s="1">
         <v>44835</v>
       </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="3"/>
       <c r="K25">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -852,7 +1061,9 @@
         <f>SUM(K$3:K25)</f>
         <v>0</v>
       </c>
-      <c r="O25">
+      <c r="M25" s="4"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="3">
         <f>SUM(N$3:N25)</f>
         <v>0</v>
       </c>
@@ -861,6 +1072,11 @@
       <c r="A26" s="1">
         <v>44866</v>
       </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="3"/>
       <c r="K26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -869,7 +1085,9 @@
         <f>SUM(K$3:K26)</f>
         <v>0</v>
       </c>
-      <c r="O26">
+      <c r="M26" s="4"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="3">
         <f>SUM(N$3:N26)</f>
         <v>0</v>
       </c>
@@ -883,5 +1101,6 @@
     <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
More small xls tweaks
</commit_message>
<xml_diff>
--- a/public/xls-template/Statistik.xlsx
+++ b/public/xls-template/Statistik.xlsx
@@ -91,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -117,11 +117,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -139,16 +170,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -433,7 +461,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -488,7 +516,7 @@
       <c r="F2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="10" t="s">
@@ -509,7 +537,7 @@
       <c r="M2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="11" t="s">
         <v>9</v>
       </c>
       <c r="O2" s="10" t="s">

</xml_diff>

<commit_message>
Info per municipality in statistics xls
</commit_message>
<xml_diff>
--- a/public/xls-template/Statistik.xlsx
+++ b/public/xls-template/Statistik.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
   </bookViews>
   <sheets>
-    <sheet name="Evikomp" sheetId="1" r:id="rId1"/>
+    <sheet name="Evikomp totalt" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -158,6 +158,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -168,15 +177,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -475,72 +475,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="7" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="5" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="6"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="9"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -563,9 +563,9 @@
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="3">
-        <f>SUM(N$3:N3)</f>
-        <v>0</v>
+      <c r="O3" s="3" t="str">
+        <f>IF(N3="","",SUM(N$3:N3))</f>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -581,15 +581,15 @@
         <f t="shared" ref="K4:K26" si="0">I4+J4</f>
         <v>0</v>
       </c>
-      <c r="L4">
-        <f>SUM(K$3:K4)</f>
-        <v>0</v>
+      <c r="L4" t="str">
+        <f>IF(SUM(K$3:K3)=SUM(K$3:K4),"",SUM(K$3:K4))</f>
+        <v/>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="3">
-        <f>SUM(N$3:N4)</f>
-        <v>0</v>
+      <c r="O4" s="3" t="str">
+        <f>IF(N4="","",SUM(N$3:N4))</f>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
@@ -605,15 +605,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L5">
-        <f>SUM(K$3:K5)</f>
-        <v>0</v>
+      <c r="L5" t="str">
+        <f>IF(SUM(K$3:K4)=SUM(K$3:K5),"",SUM(K$3:K5))</f>
+        <v/>
       </c>
       <c r="M5" s="4"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="3">
-        <f>SUM(N$3:N5)</f>
-        <v>0</v>
+      <c r="O5" s="3" t="str">
+        <f>IF(N5="","",SUM(N$3:N5))</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -629,15 +629,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6">
-        <f>SUM(K$3:K6)</f>
-        <v>0</v>
+      <c r="L6" t="str">
+        <f>IF(SUM(K$3:K5)=SUM(K$3:K6),"",SUM(K$3:K6))</f>
+        <v/>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="2"/>
-      <c r="O6" s="3">
-        <f>SUM(N$3:N6)</f>
-        <v>0</v>
+      <c r="O6" s="3" t="str">
+        <f>IF(N6="","",SUM(N$3:N6))</f>
+        <v/>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -653,15 +653,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L7">
-        <f>SUM(K$3:K7)</f>
-        <v>0</v>
+      <c r="L7" t="str">
+        <f>IF(SUM(K$3:K6)=SUM(K$3:K7),"",SUM(K$3:K7))</f>
+        <v/>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="3">
-        <f>SUM(N$3:N7)</f>
-        <v>0</v>
+      <c r="O7" s="3" t="str">
+        <f>IF(N7="","",SUM(N$3:N7))</f>
+        <v/>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -677,15 +677,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L8">
-        <f>SUM(K$3:K8)</f>
-        <v>0</v>
+      <c r="L8" t="str">
+        <f>IF(SUM(K$3:K7)=SUM(K$3:K8),"",SUM(K$3:K8))</f>
+        <v/>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="2"/>
-      <c r="O8" s="3">
-        <f>SUM(N$3:N8)</f>
-        <v>0</v>
+      <c r="O8" s="3" t="str">
+        <f>IF(N8="","",SUM(N$3:N8))</f>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -701,15 +701,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L9">
-        <f>SUM(K$3:K9)</f>
-        <v>0</v>
+      <c r="L9" t="str">
+        <f>IF(SUM(K$3:K8)=SUM(K$3:K9),"",SUM(K$3:K9))</f>
+        <v/>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="2"/>
-      <c r="O9" s="3">
-        <f>SUM(N$3:N9)</f>
-        <v>0</v>
+      <c r="O9" s="3" t="str">
+        <f>IF(N9="","",SUM(N$3:N9))</f>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -725,15 +725,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L10">
-        <f>SUM(K$3:K10)</f>
-        <v>0</v>
+      <c r="L10" t="str">
+        <f>IF(SUM(K$3:K9)=SUM(K$3:K10),"",SUM(K$3:K10))</f>
+        <v/>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="2"/>
-      <c r="O10" s="3">
-        <f>SUM(N$3:N10)</f>
-        <v>0</v>
+      <c r="O10" s="3" t="str">
+        <f>IF(N10="","",SUM(N$3:N10))</f>
+        <v/>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -749,15 +749,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L11">
-        <f>SUM(K$3:K11)</f>
-        <v>0</v>
+      <c r="L11" t="str">
+        <f>IF(SUM(K$3:K10)=SUM(K$3:K11),"",SUM(K$3:K11))</f>
+        <v/>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="2"/>
-      <c r="O11" s="3">
-        <f>SUM(N$3:N11)</f>
-        <v>0</v>
+      <c r="O11" s="3" t="str">
+        <f>IF(N11="","",SUM(N$3:N11))</f>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -773,15 +773,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12">
-        <f>SUM(K$3:K12)</f>
-        <v>0</v>
+      <c r="L12" t="str">
+        <f>IF(SUM(K$3:K11)=SUM(K$3:K12),"",SUM(K$3:K12))</f>
+        <v/>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="3">
-        <f>SUM(N$3:N12)</f>
-        <v>0</v>
+      <c r="O12" s="3" t="str">
+        <f>IF(N12="","",SUM(N$3:N12))</f>
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -797,15 +797,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13">
-        <f>SUM(K$3:K13)</f>
-        <v>0</v>
+      <c r="L13" t="str">
+        <f>IF(SUM(K$3:K12)=SUM(K$3:K13),"",SUM(K$3:K13))</f>
+        <v/>
       </c>
       <c r="M13" s="4"/>
       <c r="N13" s="2"/>
-      <c r="O13" s="3">
-        <f>SUM(N$3:N13)</f>
-        <v>0</v>
+      <c r="O13" s="3" t="str">
+        <f>IF(N13="","",SUM(N$3:N13))</f>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
@@ -821,15 +821,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14">
-        <f>SUM(K$3:K14)</f>
-        <v>0</v>
+      <c r="L14" t="str">
+        <f>IF(SUM(K$3:K13)=SUM(K$3:K14),"",SUM(K$3:K14))</f>
+        <v/>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="2"/>
-      <c r="O14" s="3">
-        <f>SUM(N$3:N14)</f>
-        <v>0</v>
+      <c r="O14" s="3" t="str">
+        <f>IF(N14="","",SUM(N$3:N14))</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -845,15 +845,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15">
-        <f>SUM(K$3:K15)</f>
-        <v>0</v>
+      <c r="L15" t="str">
+        <f>IF(SUM(K$3:K14)=SUM(K$3:K15),"",SUM(K$3:K15))</f>
+        <v/>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="2"/>
-      <c r="O15" s="3">
-        <f>SUM(N$3:N15)</f>
-        <v>0</v>
+      <c r="O15" s="3" t="str">
+        <f>IF(N15="","",SUM(N$3:N15))</f>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -869,15 +869,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L16">
-        <f>SUM(K$3:K16)</f>
-        <v>0</v>
+      <c r="L16" t="str">
+        <f>IF(SUM(K$3:K15)=SUM(K$3:K16),"",SUM(K$3:K16))</f>
+        <v/>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="2"/>
-      <c r="O16" s="3">
-        <f>SUM(N$3:N16)</f>
-        <v>0</v>
+      <c r="O16" s="3" t="str">
+        <f>IF(N16="","",SUM(N$3:N16))</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -893,15 +893,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L17">
-        <f>SUM(K$3:K17)</f>
-        <v>0</v>
+      <c r="L17" t="str">
+        <f>IF(SUM(K$3:K16)=SUM(K$3:K17),"",SUM(K$3:K17))</f>
+        <v/>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="2"/>
-      <c r="O17" s="3">
-        <f>SUM(N$3:N17)</f>
-        <v>0</v>
+      <c r="O17" s="3" t="str">
+        <f>IF(N17="","",SUM(N$3:N17))</f>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -917,15 +917,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18">
-        <f>SUM(K$3:K18)</f>
-        <v>0</v>
+      <c r="L18" t="str">
+        <f>IF(SUM(K$3:K17)=SUM(K$3:K18),"",SUM(K$3:K18))</f>
+        <v/>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="2"/>
-      <c r="O18" s="3">
-        <f>SUM(N$3:N18)</f>
-        <v>0</v>
+      <c r="O18" s="3" t="str">
+        <f>IF(N18="","",SUM(N$3:N18))</f>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -941,15 +941,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19">
-        <f>SUM(K$3:K19)</f>
-        <v>0</v>
+      <c r="L19" t="str">
+        <f>IF(SUM(K$3:K18)=SUM(K$3:K19),"",SUM(K$3:K19))</f>
+        <v/>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="2"/>
-      <c r="O19" s="3">
-        <f>SUM(N$3:N19)</f>
-        <v>0</v>
+      <c r="O19" s="3" t="str">
+        <f>IF(N19="","",SUM(N$3:N19))</f>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -965,15 +965,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L20">
-        <f>SUM(K$3:K20)</f>
-        <v>0</v>
+      <c r="L20" t="str">
+        <f>IF(SUM(K$3:K19)=SUM(K$3:K20),"",SUM(K$3:K20))</f>
+        <v/>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="2"/>
-      <c r="O20" s="3">
-        <f>SUM(N$3:N20)</f>
-        <v>0</v>
+      <c r="O20" s="3" t="str">
+        <f>IF(N20="","",SUM(N$3:N20))</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -989,15 +989,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L21">
-        <f>SUM(K$3:K21)</f>
-        <v>0</v>
+      <c r="L21" t="str">
+        <f>IF(SUM(K$3:K20)=SUM(K$3:K21),"",SUM(K$3:K21))</f>
+        <v/>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="2"/>
-      <c r="O21" s="3">
-        <f>SUM(N$3:N21)</f>
-        <v>0</v>
+      <c r="O21" s="3" t="str">
+        <f>IF(N21="","",SUM(N$3:N21))</f>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1013,15 +1013,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L22">
-        <f>SUM(K$3:K22)</f>
-        <v>0</v>
+      <c r="L22" t="str">
+        <f>IF(SUM(K$3:K21)=SUM(K$3:K22),"",SUM(K$3:K22))</f>
+        <v/>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="2"/>
-      <c r="O22" s="3">
-        <f>SUM(N$3:N22)</f>
-        <v>0</v>
+      <c r="O22" s="3" t="str">
+        <f>IF(N22="","",SUM(N$3:N22))</f>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
@@ -1037,15 +1037,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L23">
-        <f>SUM(K$3:K23)</f>
-        <v>0</v>
+      <c r="L23" t="str">
+        <f>IF(SUM(K$3:K22)=SUM(K$3:K23),"",SUM(K$3:K23))</f>
+        <v/>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="2"/>
-      <c r="O23" s="3">
-        <f>SUM(N$3:N23)</f>
-        <v>0</v>
+      <c r="O23" s="3" t="str">
+        <f>IF(N23="","",SUM(N$3:N23))</f>
+        <v/>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
@@ -1061,15 +1061,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L24">
-        <f>SUM(K$3:K24)</f>
-        <v>0</v>
+      <c r="L24" t="str">
+        <f>IF(SUM(K$3:K23)=SUM(K$3:K24),"",SUM(K$3:K24))</f>
+        <v/>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="2"/>
-      <c r="O24" s="3">
-        <f>SUM(N$3:N24)</f>
-        <v>0</v>
+      <c r="O24" s="3" t="str">
+        <f>IF(N24="","",SUM(N$3:N24))</f>
+        <v/>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
@@ -1085,15 +1085,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L25">
-        <f>SUM(K$3:K25)</f>
-        <v>0</v>
+      <c r="L25" t="str">
+        <f>IF(SUM(K$3:K24)=SUM(K$3:K25),"",SUM(K$3:K25))</f>
+        <v/>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="2"/>
-      <c r="O25" s="3">
-        <f>SUM(N$3:N25)</f>
-        <v>0</v>
+      <c r="O25" s="3" t="str">
+        <f>IF(N25="","",SUM(N$3:N25))</f>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
@@ -1115,9 +1115,9 @@
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="2"/>
-      <c r="O26" s="3">
-        <f>SUM(N$3:N26)</f>
-        <v>0</v>
+      <c r="O26" s="3" t="str">
+        <f>IF(N26="","",SUM(N$3:N26))</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>